<commit_message>
New testing db setup working. Baseclassifier builds.
</commit_message>
<xml_diff>
--- a/cytopy/tests/assets/test_panel.xlsx
+++ b/cytopy/tests/assets/test_panel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="mappings" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t xml:space="preserve">channel</t>
   </si>
@@ -57,6 +57,149 @@
   </si>
   <si>
     <t xml:space="preserve">permutations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSC\.H</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">SSC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">\.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">H</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">FL1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">\.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">H</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">FL2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">\.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">H</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">FL3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">\.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">H</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">FL4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">\.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">H</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -66,7 +209,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,6 +230,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -163,11 +311,11 @@
   </sheetPr>
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
@@ -280,11 +428,11 @@
   </sheetPr>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="46.03"/>
@@ -310,30 +458,66 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>